<commit_message>
add excel authorization and sign up
</commit_message>
<xml_diff>
--- a/UsersData.xlsx
+++ b/UsersData.xlsx
@@ -4,28 +4,38 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="540" windowWidth="13095" windowHeight="4560"/>
+    <workbookView windowHeight="7875" windowWidth="18855" xWindow="240" yWindow="555"/>
   </bookViews>
   <sheets>
-    <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>q</t>
   </si>
   <si>
-    <t>a</t>
+    <t>z</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -53,16 +63,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -71,10 +81,10 @@
   <a:themeElements>
     <a:clrScheme name="Стандартная">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -230,7 +240,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -239,13 +249,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -255,7 +265,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -264,7 +274,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -273,7 +283,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -283,12 +293,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -319,7 +329,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -338,7 +348,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -351,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -367,15 +377,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>